<commit_message>
Started event notification system.
</commit_message>
<xml_diff>
--- a/WorkBot/main/backend/ordering/OrderFiles/Hillcrest Dairy/Hillcrest Dairy_Bakery_20250322.xlsx
+++ b/WorkBot/main/backend/ordering/OrderFiles/Hillcrest Dairy/Hillcrest Dairy_Bakery_20250322.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,6 +502,114 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>wholeg</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Milk - Whole</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>16.08</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>160.80</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>skimg</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Milk - Skim</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>15.56</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>15.56</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>twog</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Milk - 2%</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>16.08</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>257.28</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>choqt</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Milk - Chocolate (9/32oz)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>17.55</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>17.55</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>